<commit_message>
Add wsm salesorder mapping.
</commit_message>
<xml_diff>
--- a/payload/wms connector/salesorder/SalesOrder mapping.xlsx
+++ b/payload/wms connector/salesorder/SalesOrder mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420"/>
+    <workbookView windowWidth="23040" windowHeight="9420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Order header" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="147">
   <si>
     <t>column type</t>
   </si>
@@ -256,7 +256,8 @@
     <t>DiscountAmount</t>
   </si>
   <si>
-    <t>Use discountamout for PromotionAmount?</t>
+    <t>Use discountamout for PromotionAmount?
+subtotalamount*discountrate+discountamount?</t>
   </si>
   <si>
     <t>PromotionAmount</t>
@@ -296,6 +297,9 @@
   </si>
   <si>
     <t>MappedShippingCarrier</t>
+  </si>
+  <si>
+    <t>wms fill up</t>
   </si>
   <si>
     <t>MappedShippingService</t>
@@ -562,8 +566,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -618,8 +622,23 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -632,25 +651,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -670,10 +690,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -694,24 +730,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -726,7 +753,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -734,29 +761,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -776,7 +780,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -797,6 +801,84 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -809,49 +891,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,19 +927,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -887,13 +945,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,43 +957,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -959,25 +981,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1021,6 +1031,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1032,15 +1066,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1069,21 +1094,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1111,10 +1121,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1123,137 +1133,137 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1278,10 +1288,25 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1634,8 +1659,8 @@
   <sheetPr/>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1643,7 +1668,7 @@
     <col min="1" max="1" width="33.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="34.7777777777778" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="34.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="22.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="47.5555555555556" customWidth="1"/>
     <col min="5" max="5" width="23.1111111111111" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="24.7777777777778" customWidth="1"/>
     <col min="7" max="7" width="40.8888888888889" customWidth="1"/>
@@ -1677,21 +1702,21 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="7" t="str">
         <f>REPLACE(E2,14,1,F2)</f>
         <v>as '{header}.SalesOrderUuid',</v>
       </c>
-      <c r="H2" s="9" t="str">
+      <c r="H2" s="11" t="str">
         <f>_xlfn.CONCAT(B2,C2," ",G2)</f>
         <v>{InfoHelper.TableAllies}.SalesOrderUuid as '{header}.SalesOrderUuid',</v>
       </c>
@@ -1721,7 +1746,7 @@
         <f>REPLACE(E3,14,1,F3)</f>
         <v>as '{header}.WarehouseCode',</v>
       </c>
-      <c r="H3" s="9" t="str">
+      <c r="H3" s="11" t="str">
         <f>_xlfn.CONCAT(B3,C3," ",G3)</f>
         <v>{InfoHelper.TableAllies}.WarehouseCode as '{header}.WarehouseCode',</v>
       </c>
@@ -1753,7 +1778,7 @@
         <f t="shared" ref="G4:G35" si="0">REPLACE(E4,14,1,F4)</f>
         <v>as '{header}.WarehouseNum',</v>
       </c>
-      <c r="H4" s="9" t="str">
+      <c r="H4" s="11" t="str">
         <f t="shared" ref="H4:H35" si="1">_xlfn.CONCAT(B4,C4," ",G4)</f>
         <v>{Helper.TableAllies}.WarehouseNum as '{header}.WarehouseNum',</v>
       </c>
@@ -1783,7 +1808,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.CentralDatabaseNum',</v>
       </c>
-      <c r="H5" s="9" t="str">
+      <c r="H5" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DatabaseNum as '{header}.CentralDatabaseNum',</v>
       </c>
@@ -1813,7 +1838,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.CentralOrderNum',</v>
       </c>
-      <c r="H6" s="9" t="str">
+      <c r="H6" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.CentralOrderNum as '{header}.CentralOrderNum',</v>
       </c>
@@ -1843,7 +1868,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelNum',</v>
       </c>
-      <c r="H7" s="9" t="str">
+      <c r="H7" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelNum as '{header}.ChannelNum',</v>
       </c>
@@ -1873,7 +1898,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelAccountNum',</v>
       </c>
-      <c r="H8" s="9" t="str">
+      <c r="H8" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelAccountNum as '{header}.ChannelAccountNum',</v>
       </c>
@@ -1903,7 +1928,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelAccountName',</v>
       </c>
-      <c r="H9" s="9" t="str">
+      <c r="H9" s="11" t="str">
         <f t="shared" si="1"/>
         <v>channelAccount.ChannelAccountName as '{header}.ChannelAccountName',</v>
       </c>
@@ -1933,7 +1958,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelOrderId',</v>
       </c>
-      <c r="H10" s="9" t="str">
+      <c r="H10" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelOrderId as '{header}.ChannelOrderId',</v>
       </c>
@@ -1963,7 +1988,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SecondaryChannelOrderId',</v>
       </c>
-      <c r="H11" s="9" t="str">
+      <c r="H11" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.SecondaryChannelOrderId as '{header}.SecondaryChannelOrderId',</v>
       </c>
@@ -1993,7 +2018,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SellerOrderId',</v>
       </c>
-      <c r="H12" s="9" t="str">
+      <c r="H12" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.OrderNumber as '{header}.SellerOrderId',</v>
       </c>
@@ -2023,7 +2048,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.Currency',</v>
       </c>
-      <c r="H13" s="9" t="str">
+      <c r="H13" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.Currency as '{header}.Currency',</v>
       </c>
@@ -2053,7 +2078,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.OriginalOrderDate',</v>
       </c>
-      <c r="H14" s="9" t="str">
+      <c r="H14" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.OrderDate as '{header}.OriginalOrderDate',</v>
       </c>
@@ -2085,7 +2110,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SellerPublicNotes',</v>
       </c>
-      <c r="H15" s="9" t="str">
+      <c r="H15" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.SellerPublicNotes as '{header}.SellerPublicNotes',</v>
       </c>
@@ -2115,7 +2140,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SellerPrivateNotes',</v>
       </c>
-      <c r="H16" s="9" t="str">
+      <c r="H16" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.Notes as '{header}.SellerPrivateNotes',</v>
       </c>
@@ -2147,7 +2172,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.EndBuyerInstruction',</v>
       </c>
-      <c r="H17" s="9" t="str">
+      <c r="H17" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EndBuyerInstruction as '{header}.EndBuyerInstruction',</v>
       </c>
@@ -2177,7 +2202,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalOrderAmount',</v>
       </c>
-      <c r="H18" s="9" t="str">
+      <c r="H18" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalAmount as '{header}.TotalOrderAmount',</v>
       </c>
@@ -2207,7 +2232,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalTaxAmount',</v>
       </c>
-      <c r="H19" s="9" t="str">
+      <c r="H19" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TaxAmount as '{header}.TotalTaxAmount',</v>
       </c>
@@ -2237,7 +2262,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingAmount',</v>
       </c>
-      <c r="H20" s="9" t="str">
+      <c r="H20" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.ShippingAmount as '{header}.TotalShippingAmount',</v>
       </c>
@@ -2267,7 +2292,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingTaxAmount',</v>
       </c>
-      <c r="H21" s="9" t="str">
+      <c r="H21" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.ShippingTaxAmount as '{header}.TotalShippingTaxAmount',</v>
       </c>
@@ -2299,7 +2324,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingDiscount',</v>
       </c>
-      <c r="H22" s="9" t="str">
+      <c r="H22" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalShippingDiscount as '{header}.TotalShippingDiscount',</v>
       </c>
@@ -2331,7 +2356,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingDiscountTaxAmount',</v>
       </c>
-      <c r="H23" s="9" t="str">
+      <c r="H23" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalShippingDiscountTaxAmount as '{header}.TotalShippingDiscountTaxAmount',</v>
       </c>
@@ -2363,7 +2388,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalInsuranceAmount',</v>
       </c>
-      <c r="H24" s="9" t="str">
+      <c r="H24" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalInsuranceAmount as '{header}.TotalInsuranceAmount',</v>
       </c>
@@ -2395,7 +2420,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalGiftOptionAmount',</v>
       </c>
-      <c r="H25" s="9" t="str">
+      <c r="H25" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalGiftOptionAmount as '{header}.TotalGiftOptionAmount',</v>
       </c>
@@ -2427,7 +2452,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalGiftOptionTaxAmount',</v>
       </c>
-      <c r="H26" s="9" t="str">
+      <c r="H26" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalGiftOptionTaxAmount as '{header}.TotalGiftOptionTaxAmount',</v>
       </c>
@@ -2459,7 +2484,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.AdditionalCostOrDiscount',</v>
       </c>
-      <c r="H27" s="9" t="str">
+      <c r="H27" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.AdditionalCostOrDiscount as '{header}.AdditionalCostOrDiscount',</v>
       </c>
@@ -2468,37 +2493,37 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" ht="25.2" customHeight="1" spans="1:10">
-      <c r="A28" s="2" t="s">
+    <row r="28" s="9" customFormat="1" ht="25.2" customHeight="1" spans="1:10">
+      <c r="A28" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="7" t="s">
+      <c r="E28" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="7" t="str">
+      <c r="G28" s="13" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.PromotionAmount',</v>
       </c>
-      <c r="H28" s="9" t="str">
+      <c r="H28" s="14" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DiscountAmount as '{header}.PromotionAmount',</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="2"/>
+      <c r="J28" s="12"/>
     </row>
     <row r="29" ht="37.8" customHeight="1" spans="1:10">
       <c r="A29" s="2" t="s">
@@ -2523,7 +2548,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.EstimatedShipDate',</v>
       </c>
-      <c r="H29" s="9" t="str">
+      <c r="H29" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EstimatedShipDate as '{header}.EstimatedShipDate',</v>
       </c>
@@ -2555,7 +2580,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.EarliestShipDate',</v>
       </c>
-      <c r="H30" s="9" t="str">
+      <c r="H30" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EarliestShipDate as '{header}.EarliestShipDate',</v>
       </c>
@@ -2574,9 +2599,7 @@
       <c r="C31" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="D31" s="5"/>
       <c r="E31" s="7" t="s">
         <v>8</v>
       </c>
@@ -2587,7 +2610,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.LatestShipDate',</v>
       </c>
-      <c r="H31" s="9" t="str">
+      <c r="H31" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.LatestShipDate as '{header}.LatestShipDate',</v>
       </c>
@@ -2606,9 +2629,7 @@
       <c r="C32" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>55</v>
-      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="7" t="s">
         <v>8</v>
       </c>
@@ -2619,7 +2640,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.DeliverByDate',</v>
       </c>
-      <c r="H32" s="9" t="str">
+      <c r="H32" s="11" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DeliverByDate as '{header}.DeliverByDate',</v>
       </c>
@@ -2628,133 +2649,133 @@
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="5" t="s">
+    <row r="33" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A33" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="7" t="s">
+      <c r="E33" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="7" t="str">
+      <c r="G33" s="13" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.RequestShippingCarrier',</v>
       </c>
-      <c r="H33" s="9" t="str">
+      <c r="H33" s="14" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ShippingCarrier as '{header}.RequestShippingCarrier',</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="I33" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="12"/>
+    </row>
+    <row r="34" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A34" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="7" t="s">
+      <c r="E34" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="7" t="str">
+      <c r="G34" s="13" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.RequestShippingService',</v>
       </c>
-      <c r="H34" s="9" t="str">
+      <c r="H34" s="14" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ShippingClass as '{header}.RequestShippingService',</v>
       </c>
-      <c r="I34" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="I34" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="12"/>
+    </row>
+    <row r="35" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="7" t="s">
+      <c r="D35" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="7" t="str">
+      <c r="G35" s="13" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.MappedShippingCarrier',</v>
       </c>
-      <c r="H35" s="9" t="str">
+      <c r="H35" s="14" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.MappedShippingCarrier as '{header}.MappedShippingCarrier',</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="I35" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="12"/>
+    </row>
+    <row r="36" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A36" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G36" s="7" t="str">
+      <c r="E36" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G36" s="13" t="str">
         <f t="shared" ref="G36:G78" si="2">REPLACE(E36,14,1,F36)</f>
         <v>as '{header}.MappedShippingService',</v>
       </c>
-      <c r="H36" s="9" t="str">
+      <c r="H36" s="14" t="str">
         <f t="shared" ref="H36:H78" si="3">_xlfn.CONCAT(B36,C36," ",G36)</f>
         <v>{Helper.TableAllies}.MappedShippingService as '{header}.MappedShippingService',</v>
       </c>
-      <c r="I36" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="2"/>
+      <c r="I36" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="12"/>
     </row>
     <row r="37" ht="25.2" customHeight="1" spans="1:10">
       <c r="A37" s="2" t="s">
@@ -2764,20 +2785,20 @@
         <v>6</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G37" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToName',</v>
       </c>
-      <c r="H37" s="9" t="str">
+      <c r="H37" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToName as '{header}.ShipToName',</v>
       </c>
@@ -2794,20 +2815,20 @@
         <v>6</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G38" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToFirstName',</v>
       </c>
-      <c r="H38" s="9" t="str">
+      <c r="H38" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToFirstName as '{header}.ShipToFirstName',</v>
       </c>
@@ -2824,20 +2845,20 @@
         <v>6</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G39" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToLastName',</v>
       </c>
-      <c r="H39" s="9" t="str">
+      <c r="H39" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToLastName as '{header}.ShipToLastName',</v>
       </c>
@@ -2854,20 +2875,20 @@
         <v>6</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G40" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToSuffix',</v>
       </c>
-      <c r="H40" s="9" t="str">
+      <c r="H40" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToSuffix as '{header}.ShipToSuffix',</v>
       </c>
@@ -2884,20 +2905,20 @@
         <v>6</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G41" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCompany',</v>
       </c>
-      <c r="H41" s="9" t="str">
+      <c r="H41" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCompany as '{header}.ShipToCompany',</v>
       </c>
@@ -2914,20 +2935,20 @@
         <v>6</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G42" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCompanyJobTitle',</v>
       </c>
-      <c r="H42" s="9" t="str">
+      <c r="H42" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCompanyJobTitle as '{header}.ShipToCompanyJobTitle',</v>
       </c>
@@ -2944,20 +2965,20 @@
         <v>6</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G43" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAttention',</v>
       </c>
-      <c r="H43" s="9" t="str">
+      <c r="H43" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAttention as '{header}.ShipToAttention',</v>
       </c>
@@ -2974,20 +2995,20 @@
         <v>6</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G44" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToDaytimePhone',</v>
       </c>
-      <c r="H44" s="9" t="str">
+      <c r="H44" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToDaytimePhone as '{header}.ShipToDaytimePhone',</v>
       </c>
@@ -3004,20 +3025,20 @@
         <v>6</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G45" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToNightPhone',</v>
       </c>
-      <c r="H45" s="9" t="str">
+      <c r="H45" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToNightPhone as '{header}.ShipToNightPhone',</v>
       </c>
@@ -3034,20 +3055,20 @@
         <v>6</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G46" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAddressLine1',</v>
       </c>
-      <c r="H46" s="9" t="str">
+      <c r="H46" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine1 as '{header}.ShipToAddressLine1',</v>
       </c>
@@ -3064,20 +3085,20 @@
         <v>6</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G47" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAddressLine2',</v>
       </c>
-      <c r="H47" s="9" t="str">
+      <c r="H47" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine2 as '{header}.ShipToAddressLine2',</v>
       </c>
@@ -3094,20 +3115,20 @@
         <v>6</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G48" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAddressLine3',</v>
       </c>
-      <c r="H48" s="9" t="str">
+      <c r="H48" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine3 as '{header}.ShipToAddressLine3',</v>
       </c>
@@ -3124,20 +3145,20 @@
         <v>6</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G49" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCity',</v>
       </c>
-      <c r="H49" s="9" t="str">
+      <c r="H49" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCity as '{header}.ShipToCity',</v>
       </c>
@@ -3154,20 +3175,20 @@
         <v>6</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G50" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToState',</v>
       </c>
-      <c r="H50" s="9" t="str">
+      <c r="H50" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToState as '{header}.ShipToState',</v>
       </c>
@@ -3184,20 +3205,20 @@
         <v>6</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G51" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToStateFullName',</v>
       </c>
-      <c r="H51" s="9" t="str">
+      <c r="H51" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToStateFullName as '{header}.ShipToStateFullName',</v>
       </c>
@@ -3214,20 +3235,20 @@
         <v>6</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G52" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToPostalCode',</v>
       </c>
-      <c r="H52" s="9" t="str">
+      <c r="H52" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToPostalCode as '{header}.ShipToPostalCode',</v>
       </c>
@@ -3244,20 +3265,20 @@
         <v>6</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G53" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToPostalCodeExt',</v>
       </c>
-      <c r="H53" s="9" t="str">
+      <c r="H53" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToPostalCodeExt as '{header}.ShipToPostalCodeExt',</v>
       </c>
@@ -3274,20 +3295,20 @@
         <v>6</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G54" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCounty',</v>
       </c>
-      <c r="H54" s="9" t="str">
+      <c r="H54" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCounty as '{header}.ShipToCounty',</v>
       </c>
@@ -3304,20 +3325,20 @@
         <v>6</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G55" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCountry',</v>
       </c>
-      <c r="H55" s="9" t="str">
+      <c r="H55" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCountry as '{header}.ShipToCountry',</v>
       </c>
@@ -3334,20 +3355,20 @@
         <v>6</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G56" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToEmail',</v>
       </c>
-      <c r="H56" s="9" t="str">
+      <c r="H56" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToEmail as '{header}.ShipToEmail',</v>
       </c>
@@ -3364,20 +3385,20 @@
         <v>6</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G57" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToName',</v>
       </c>
-      <c r="H57" s="9" t="str">
+      <c r="H57" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToName as '{header}.BillToName',</v>
       </c>
@@ -3394,20 +3415,20 @@
         <v>6</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G58" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToFirstName',</v>
       </c>
-      <c r="H58" s="9" t="str">
+      <c r="H58" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToFirstName as '{header}.BillToFirstName',</v>
       </c>
@@ -3424,20 +3445,20 @@
         <v>6</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G59" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToLastName',</v>
       </c>
-      <c r="H59" s="9" t="str">
+      <c r="H59" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToLastName as '{header}.BillToLastName',</v>
       </c>
@@ -3454,20 +3475,20 @@
         <v>6</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G60" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToSuffix',</v>
       </c>
-      <c r="H60" s="9" t="str">
+      <c r="H60" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToSuffix as '{header}.BillToSuffix',</v>
       </c>
@@ -3484,20 +3505,20 @@
         <v>6</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G61" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCompany',</v>
       </c>
-      <c r="H61" s="9" t="str">
+      <c r="H61" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCompany as '{header}.BillToCompany',</v>
       </c>
@@ -3514,20 +3535,20 @@
         <v>6</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G62" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCompanyJobTitle',</v>
       </c>
-      <c r="H62" s="9" t="str">
+      <c r="H62" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCompanyJobTitle as '{header}.BillToCompanyJobTitle',</v>
       </c>
@@ -3544,20 +3565,20 @@
         <v>6</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G63" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAttention',</v>
       </c>
-      <c r="H63" s="9" t="str">
+      <c r="H63" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAttention as '{header}.BillToAttention',</v>
       </c>
@@ -3574,20 +3595,20 @@
         <v>6</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G64" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAddressLine1',</v>
       </c>
-      <c r="H64" s="9" t="str">
+      <c r="H64" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine1 as '{header}.BillToAddressLine1',</v>
       </c>
@@ -3604,20 +3625,20 @@
         <v>6</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G65" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAddressLine2',</v>
       </c>
-      <c r="H65" s="9" t="str">
+      <c r="H65" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine2 as '{header}.BillToAddressLine2',</v>
       </c>
@@ -3634,20 +3655,20 @@
         <v>6</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G66" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAddressLine3',</v>
       </c>
-      <c r="H66" s="9" t="str">
+      <c r="H66" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine3 as '{header}.BillToAddressLine3',</v>
       </c>
@@ -3664,20 +3685,20 @@
         <v>6</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G67" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCity',</v>
       </c>
-      <c r="H67" s="9" t="str">
+      <c r="H67" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCity as '{header}.BillToCity',</v>
       </c>
@@ -3694,20 +3715,20 @@
         <v>6</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G68" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToState',</v>
       </c>
-      <c r="H68" s="9" t="str">
+      <c r="H68" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToState as '{header}.BillToState',</v>
       </c>
@@ -3724,20 +3745,20 @@
         <v>6</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G69" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToStateFullName',</v>
       </c>
-      <c r="H69" s="9" t="str">
+      <c r="H69" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToStateFullName as '{header}.BillToStateFullName',</v>
       </c>
@@ -3754,20 +3775,20 @@
         <v>6</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G70" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToPostalCode',</v>
       </c>
-      <c r="H70" s="9" t="str">
+      <c r="H70" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToPostalCode as '{header}.BillToPostalCode',</v>
       </c>
@@ -3784,20 +3805,20 @@
         <v>6</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G71" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToPostalCodeExt',</v>
       </c>
-      <c r="H71" s="9" t="str">
+      <c r="H71" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToPostalCodeExt as '{header}.BillToPostalCodeExt',</v>
       </c>
@@ -3814,20 +3835,20 @@
         <v>6</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G72" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCounty',</v>
       </c>
-      <c r="H72" s="9" t="str">
+      <c r="H72" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCounty as '{header}.BillToCounty',</v>
       </c>
@@ -3844,20 +3865,20 @@
         <v>6</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G73" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCountry',</v>
       </c>
-      <c r="H73" s="9" t="str">
+      <c r="H73" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCountry as '{header}.BillToCountry',</v>
       </c>
@@ -3874,20 +3895,20 @@
         <v>6</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G74" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToEmail',</v>
       </c>
-      <c r="H74" s="9" t="str">
+      <c r="H74" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToEmail as '{header}.BillToEmail',</v>
       </c>
@@ -3904,20 +3925,20 @@
         <v>6</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G75" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToDaytimePhone',</v>
       </c>
-      <c r="H75" s="9" t="str">
+      <c r="H75" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToDaytimePhone as '{header}.BillToDaytimePhone',</v>
       </c>
@@ -3934,20 +3955,20 @@
         <v>6</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G76" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.BillToNightPhone',</v>
       </c>
-      <c r="H76" s="9" t="str">
+      <c r="H76" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToNightPhone as '{header}.BillToNightPhone',</v>
       </c>
@@ -3964,7 +3985,7 @@
         <v>11</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>13</v>
@@ -3973,13 +3994,13 @@
         <v>8</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G77" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.SignatureFlag',</v>
       </c>
-      <c r="H77" s="9" t="str">
+      <c r="H77" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{Helper.TableAllies}.SignatureFlag as '{header}.SignatureFlag',</v>
       </c>
@@ -3996,22 +4017,22 @@
         <v>11</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D78" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F78" s="7" t="s">
         <v>109</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="G78" s="7" t="str">
         <f t="shared" si="2"/>
         <v>as '{header}.ShipmentCount',</v>
       </c>
-      <c r="H78" s="9" t="str">
+      <c r="H78" s="11" t="str">
         <f t="shared" si="3"/>
         <v>{Helper.TableAllies}.ShipmentCount as '{header}.ShipmentCount',</v>
       </c>
@@ -4113,8 +4134,8 @@
   <sheetPr/>
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -4150,7 +4171,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -4159,19 +4180,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G3" t="str">
         <f>REPLACE(E3,12,1,F3)</f>
@@ -4187,7 +4208,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>15</v>
@@ -4196,7 +4217,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>15</v>
@@ -4215,19 +4236,19 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>113</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -4243,19 +4264,19 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -4271,19 +4292,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -4299,16 +4320,16 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -4324,19 +4345,19 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -4352,16 +4373,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="0"/>
@@ -4377,16 +4398,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
@@ -4403,16 +4424,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
@@ -4428,19 +4449,19 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
@@ -4456,16 +4477,16 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
@@ -4481,16 +4502,16 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
@@ -4506,16 +4527,16 @@
         <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -4531,19 +4552,19 @@
         <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
@@ -4559,19 +4580,19 @@
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -4587,19 +4608,19 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
@@ -4615,19 +4636,19 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
@@ -4643,19 +4664,19 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
@@ -4671,19 +4692,19 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
@@ -4699,19 +4720,19 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
@@ -4727,19 +4748,19 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
@@ -4755,19 +4776,19 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
@@ -4783,19 +4804,19 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -4811,19 +4832,19 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>141</v>
+        <v>112</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>142</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
@@ -4839,19 +4860,19 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
@@ -4867,19 +4888,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Add open s/o mapping
</commit_message>
<xml_diff>
--- a/payload/wms connector/salesorder/SalesOrder mapping.xlsx
+++ b/payload/wms connector/salesorder/SalesOrder mapping.xlsx
@@ -12,14 +12,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Order header'!$D$1:$D$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">orderitem!$D$1:$D$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">orderitem!$B$1:$B$30</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="146">
   <si>
     <t>column type</t>
   </si>
@@ -462,18 +462,18 @@
     <t>OriginalLineId</t>
   </si>
   <si>
-    <t>as '{item}. ',</t>
-  </si>
-  <si>
-    <t>Seq</t>
-  </si>
-  <si>
-    <t>Seq as CentralOrderLineNum?</t>
+    <t>as ' ',</t>
+  </si>
+  <si>
+    <t>{OrderLineHelper.TableAllies}.</t>
   </si>
   <si>
     <t>CentralOrderLineNum</t>
   </si>
   <si>
+    <t>{ProdcutHelper.TableAllies}.</t>
+  </si>
+  <si>
     <t>CentralProductNum</t>
   </si>
   <si>
@@ -483,6 +483,9 @@
     <t>SKU</t>
   </si>
   <si>
+    <t>UPC</t>
+  </si>
+  <si>
     <t>ItemTitle</t>
   </si>
   <si>
@@ -496,12 +499,6 @@
   </si>
   <si>
     <t>CancelQty</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>price as unitprice?</t>
   </si>
   <si>
     <t>UnitPrice</t>
@@ -566,9 +563,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
@@ -622,6 +619,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -638,39 +657,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -692,9 +681,17 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -702,14 +699,6 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -730,8 +719,23 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -739,13 +743,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -760,7 +757,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -780,7 +777,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -801,7 +798,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -819,7 +822,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -831,19 +834,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,55 +906,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -921,13 +924,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -939,13 +960,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,37 +972,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1016,6 +1007,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1027,6 +1027,36 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1055,45 +1085,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1121,10 +1112,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1133,137 +1124,137 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1288,7 +1279,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
@@ -1702,21 +1696,21 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="7" t="str">
         <f>REPLACE(E2,14,1,F2)</f>
         <v>as '{header}.SalesOrderUuid',</v>
       </c>
-      <c r="H2" s="11" t="str">
+      <c r="H2" s="12" t="str">
         <f>_xlfn.CONCAT(B2,C2," ",G2)</f>
         <v>{InfoHelper.TableAllies}.SalesOrderUuid as '{header}.SalesOrderUuid',</v>
       </c>
@@ -1746,7 +1740,7 @@
         <f>REPLACE(E3,14,1,F3)</f>
         <v>as '{header}.WarehouseCode',</v>
       </c>
-      <c r="H3" s="11" t="str">
+      <c r="H3" s="12" t="str">
         <f>_xlfn.CONCAT(B3,C3," ",G3)</f>
         <v>{InfoHelper.TableAllies}.WarehouseCode as '{header}.WarehouseCode',</v>
       </c>
@@ -1778,7 +1772,7 @@
         <f t="shared" ref="G4:G35" si="0">REPLACE(E4,14,1,F4)</f>
         <v>as '{header}.WarehouseNum',</v>
       </c>
-      <c r="H4" s="11" t="str">
+      <c r="H4" s="12" t="str">
         <f t="shared" ref="H4:H35" si="1">_xlfn.CONCAT(B4,C4," ",G4)</f>
         <v>{Helper.TableAllies}.WarehouseNum as '{header}.WarehouseNum',</v>
       </c>
@@ -1808,7 +1802,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.CentralDatabaseNum',</v>
       </c>
-      <c r="H5" s="11" t="str">
+      <c r="H5" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DatabaseNum as '{header}.CentralDatabaseNum',</v>
       </c>
@@ -1838,7 +1832,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.CentralOrderNum',</v>
       </c>
-      <c r="H6" s="11" t="str">
+      <c r="H6" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.CentralOrderNum as '{header}.CentralOrderNum',</v>
       </c>
@@ -1868,7 +1862,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelNum',</v>
       </c>
-      <c r="H7" s="11" t="str">
+      <c r="H7" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelNum as '{header}.ChannelNum',</v>
       </c>
@@ -1898,7 +1892,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelAccountNum',</v>
       </c>
-      <c r="H8" s="11" t="str">
+      <c r="H8" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelAccountNum as '{header}.ChannelAccountNum',</v>
       </c>
@@ -1928,7 +1922,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelAccountName',</v>
       </c>
-      <c r="H9" s="11" t="str">
+      <c r="H9" s="12" t="str">
         <f t="shared" si="1"/>
         <v>channelAccount.ChannelAccountName as '{header}.ChannelAccountName',</v>
       </c>
@@ -1958,7 +1952,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.ChannelOrderId',</v>
       </c>
-      <c r="H10" s="11" t="str">
+      <c r="H10" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelOrderId as '{header}.ChannelOrderId',</v>
       </c>
@@ -1988,7 +1982,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SecondaryChannelOrderId',</v>
       </c>
-      <c r="H11" s="11" t="str">
+      <c r="H11" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.SecondaryChannelOrderId as '{header}.SecondaryChannelOrderId',</v>
       </c>
@@ -2018,7 +2012,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SellerOrderId',</v>
       </c>
-      <c r="H12" s="11" t="str">
+      <c r="H12" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.OrderNumber as '{header}.SellerOrderId',</v>
       </c>
@@ -2048,7 +2042,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.Currency',</v>
       </c>
-      <c r="H13" s="11" t="str">
+      <c r="H13" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.Currency as '{header}.Currency',</v>
       </c>
@@ -2078,7 +2072,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.OriginalOrderDate',</v>
       </c>
-      <c r="H14" s="11" t="str">
+      <c r="H14" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.OrderDate as '{header}.OriginalOrderDate',</v>
       </c>
@@ -2110,7 +2104,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SellerPublicNotes',</v>
       </c>
-      <c r="H15" s="11" t="str">
+      <c r="H15" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.SellerPublicNotes as '{header}.SellerPublicNotes',</v>
       </c>
@@ -2140,7 +2134,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.SellerPrivateNotes',</v>
       </c>
-      <c r="H16" s="11" t="str">
+      <c r="H16" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.Notes as '{header}.SellerPrivateNotes',</v>
       </c>
@@ -2172,7 +2166,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.EndBuyerInstruction',</v>
       </c>
-      <c r="H17" s="11" t="str">
+      <c r="H17" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EndBuyerInstruction as '{header}.EndBuyerInstruction',</v>
       </c>
@@ -2202,7 +2196,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalOrderAmount',</v>
       </c>
-      <c r="H18" s="11" t="str">
+      <c r="H18" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalAmount as '{header}.TotalOrderAmount',</v>
       </c>
@@ -2232,7 +2226,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalTaxAmount',</v>
       </c>
-      <c r="H19" s="11" t="str">
+      <c r="H19" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TaxAmount as '{header}.TotalTaxAmount',</v>
       </c>
@@ -2262,7 +2256,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingAmount',</v>
       </c>
-      <c r="H20" s="11" t="str">
+      <c r="H20" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.ShippingAmount as '{header}.TotalShippingAmount',</v>
       </c>
@@ -2292,7 +2286,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingTaxAmount',</v>
       </c>
-      <c r="H21" s="11" t="str">
+      <c r="H21" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.ShippingTaxAmount as '{header}.TotalShippingTaxAmount',</v>
       </c>
@@ -2324,7 +2318,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingDiscount',</v>
       </c>
-      <c r="H22" s="11" t="str">
+      <c r="H22" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalShippingDiscount as '{header}.TotalShippingDiscount',</v>
       </c>
@@ -2356,7 +2350,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalShippingDiscountTaxAmount',</v>
       </c>
-      <c r="H23" s="11" t="str">
+      <c r="H23" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalShippingDiscountTaxAmount as '{header}.TotalShippingDiscountTaxAmount',</v>
       </c>
@@ -2388,7 +2382,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalInsuranceAmount',</v>
       </c>
-      <c r="H24" s="11" t="str">
+      <c r="H24" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalInsuranceAmount as '{header}.TotalInsuranceAmount',</v>
       </c>
@@ -2420,7 +2414,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalGiftOptionAmount',</v>
       </c>
-      <c r="H25" s="11" t="str">
+      <c r="H25" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalGiftOptionAmount as '{header}.TotalGiftOptionAmount',</v>
       </c>
@@ -2452,7 +2446,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.TotalGiftOptionTaxAmount',</v>
       </c>
-      <c r="H26" s="11" t="str">
+      <c r="H26" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalGiftOptionTaxAmount as '{header}.TotalGiftOptionTaxAmount',</v>
       </c>
@@ -2484,7 +2478,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.AdditionalCostOrDiscount',</v>
       </c>
-      <c r="H27" s="11" t="str">
+      <c r="H27" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.AdditionalCostOrDiscount as '{header}.AdditionalCostOrDiscount',</v>
       </c>
@@ -2493,37 +2487,37 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" s="9" customFormat="1" ht="25.2" customHeight="1" spans="1:10">
-      <c r="A28" s="12" t="s">
+    <row r="28" s="10" customFormat="1" ht="25.2" customHeight="1" spans="1:10">
+      <c r="A28" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="13" t="s">
+      <c r="E28" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="13" t="str">
+      <c r="G28" s="14" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.PromotionAmount',</v>
       </c>
-      <c r="H28" s="14" t="str">
+      <c r="H28" s="15" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DiscountAmount as '{header}.PromotionAmount',</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="I28" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J28" s="12"/>
+      <c r="J28" s="13"/>
     </row>
     <row r="29" ht="37.8" customHeight="1" spans="1:10">
       <c r="A29" s="2" t="s">
@@ -2548,7 +2542,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.EstimatedShipDate',</v>
       </c>
-      <c r="H29" s="11" t="str">
+      <c r="H29" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EstimatedShipDate as '{header}.EstimatedShipDate',</v>
       </c>
@@ -2580,7 +2574,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.EarliestShipDate',</v>
       </c>
-      <c r="H30" s="11" t="str">
+      <c r="H30" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EarliestShipDate as '{header}.EarliestShipDate',</v>
       </c>
@@ -2610,7 +2604,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.LatestShipDate',</v>
       </c>
-      <c r="H31" s="11" t="str">
+      <c r="H31" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.LatestShipDate as '{header}.LatestShipDate',</v>
       </c>
@@ -2640,7 +2634,7 @@
         <f t="shared" si="0"/>
         <v>as '{header}.DeliverByDate',</v>
       </c>
-      <c r="H32" s="11" t="str">
+      <c r="H32" s="12" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DeliverByDate as '{header}.DeliverByDate',</v>
       </c>
@@ -2649,133 +2643,133 @@
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A33" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="13" t="s">
+    <row r="33" s="10" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A33" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="13" t="s">
+      <c r="E33" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="13" t="str">
+      <c r="G33" s="14" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.RequestShippingCarrier',</v>
       </c>
-      <c r="H33" s="14" t="str">
+      <c r="H33" s="15" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ShippingCarrier as '{header}.RequestShippingCarrier',</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" s="12"/>
-    </row>
-    <row r="34" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A34" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="13" t="s">
+      <c r="I33" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="13"/>
+    </row>
+    <row r="34" s="10" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="D34" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="13" t="s">
+      <c r="E34" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="13" t="str">
+      <c r="G34" s="14" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.RequestShippingService',</v>
       </c>
-      <c r="H34" s="14" t="str">
+      <c r="H34" s="15" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ShippingClass as '{header}.RequestShippingService',</v>
       </c>
-      <c r="I34" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" s="12"/>
-    </row>
-    <row r="35" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A35" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="9" t="s">
+      <c r="I34" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" s="10" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A35" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="13" t="s">
+      <c r="E35" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="13" t="str">
+      <c r="G35" s="14" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.MappedShippingCarrier',</v>
       </c>
-      <c r="H35" s="14" t="str">
+      <c r="H35" s="15" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.MappedShippingCarrier as '{header}.MappedShippingCarrier',</v>
       </c>
-      <c r="I35" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="12"/>
-    </row>
-    <row r="36" s="9" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A36" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="9" t="s">
+      <c r="I35" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" s="10" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
+      <c r="A36" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E36" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="13" t="s">
+      <c r="E36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="13" t="str">
+      <c r="G36" s="14" t="str">
         <f t="shared" ref="G36:G78" si="2">REPLACE(E36,14,1,F36)</f>
         <v>as '{header}.MappedShippingService',</v>
       </c>
-      <c r="H36" s="14" t="str">
+      <c r="H36" s="15" t="str">
         <f t="shared" ref="H36:H78" si="3">_xlfn.CONCAT(B36,C36," ",G36)</f>
         <v>{Helper.TableAllies}.MappedShippingService as '{header}.MappedShippingService',</v>
       </c>
-      <c r="I36" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="12"/>
+      <c r="I36" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="13"/>
     </row>
     <row r="37" ht="25.2" customHeight="1" spans="1:10">
       <c r="A37" s="2" t="s">
@@ -2798,7 +2792,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToName',</v>
       </c>
-      <c r="H37" s="11" t="str">
+      <c r="H37" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToName as '{header}.ShipToName',</v>
       </c>
@@ -2828,7 +2822,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToFirstName',</v>
       </c>
-      <c r="H38" s="11" t="str">
+      <c r="H38" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToFirstName as '{header}.ShipToFirstName',</v>
       </c>
@@ -2858,7 +2852,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToLastName',</v>
       </c>
-      <c r="H39" s="11" t="str">
+      <c r="H39" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToLastName as '{header}.ShipToLastName',</v>
       </c>
@@ -2888,7 +2882,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToSuffix',</v>
       </c>
-      <c r="H40" s="11" t="str">
+      <c r="H40" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToSuffix as '{header}.ShipToSuffix',</v>
       </c>
@@ -2918,7 +2912,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCompany',</v>
       </c>
-      <c r="H41" s="11" t="str">
+      <c r="H41" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCompany as '{header}.ShipToCompany',</v>
       </c>
@@ -2948,7 +2942,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCompanyJobTitle',</v>
       </c>
-      <c r="H42" s="11" t="str">
+      <c r="H42" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCompanyJobTitle as '{header}.ShipToCompanyJobTitle',</v>
       </c>
@@ -2978,7 +2972,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAttention',</v>
       </c>
-      <c r="H43" s="11" t="str">
+      <c r="H43" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAttention as '{header}.ShipToAttention',</v>
       </c>
@@ -3008,7 +3002,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToDaytimePhone',</v>
       </c>
-      <c r="H44" s="11" t="str">
+      <c r="H44" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToDaytimePhone as '{header}.ShipToDaytimePhone',</v>
       </c>
@@ -3038,7 +3032,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToNightPhone',</v>
       </c>
-      <c r="H45" s="11" t="str">
+      <c r="H45" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToNightPhone as '{header}.ShipToNightPhone',</v>
       </c>
@@ -3068,7 +3062,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAddressLine1',</v>
       </c>
-      <c r="H46" s="11" t="str">
+      <c r="H46" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine1 as '{header}.ShipToAddressLine1',</v>
       </c>
@@ -3098,7 +3092,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAddressLine2',</v>
       </c>
-      <c r="H47" s="11" t="str">
+      <c r="H47" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine2 as '{header}.ShipToAddressLine2',</v>
       </c>
@@ -3128,7 +3122,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToAddressLine3',</v>
       </c>
-      <c r="H48" s="11" t="str">
+      <c r="H48" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine3 as '{header}.ShipToAddressLine3',</v>
       </c>
@@ -3158,7 +3152,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCity',</v>
       </c>
-      <c r="H49" s="11" t="str">
+      <c r="H49" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCity as '{header}.ShipToCity',</v>
       </c>
@@ -3188,7 +3182,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToState',</v>
       </c>
-      <c r="H50" s="11" t="str">
+      <c r="H50" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToState as '{header}.ShipToState',</v>
       </c>
@@ -3218,7 +3212,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToStateFullName',</v>
       </c>
-      <c r="H51" s="11" t="str">
+      <c r="H51" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToStateFullName as '{header}.ShipToStateFullName',</v>
       </c>
@@ -3248,7 +3242,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToPostalCode',</v>
       </c>
-      <c r="H52" s="11" t="str">
+      <c r="H52" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToPostalCode as '{header}.ShipToPostalCode',</v>
       </c>
@@ -3278,7 +3272,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToPostalCodeExt',</v>
       </c>
-      <c r="H53" s="11" t="str">
+      <c r="H53" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToPostalCodeExt as '{header}.ShipToPostalCodeExt',</v>
       </c>
@@ -3308,7 +3302,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCounty',</v>
       </c>
-      <c r="H54" s="11" t="str">
+      <c r="H54" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCounty as '{header}.ShipToCounty',</v>
       </c>
@@ -3338,7 +3332,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToCountry',</v>
       </c>
-      <c r="H55" s="11" t="str">
+      <c r="H55" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCountry as '{header}.ShipToCountry',</v>
       </c>
@@ -3368,7 +3362,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipToEmail',</v>
       </c>
-      <c r="H56" s="11" t="str">
+      <c r="H56" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToEmail as '{header}.ShipToEmail',</v>
       </c>
@@ -3398,7 +3392,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToName',</v>
       </c>
-      <c r="H57" s="11" t="str">
+      <c r="H57" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToName as '{header}.BillToName',</v>
       </c>
@@ -3428,7 +3422,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToFirstName',</v>
       </c>
-      <c r="H58" s="11" t="str">
+      <c r="H58" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToFirstName as '{header}.BillToFirstName',</v>
       </c>
@@ -3458,7 +3452,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToLastName',</v>
       </c>
-      <c r="H59" s="11" t="str">
+      <c r="H59" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToLastName as '{header}.BillToLastName',</v>
       </c>
@@ -3488,7 +3482,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToSuffix',</v>
       </c>
-      <c r="H60" s="11" t="str">
+      <c r="H60" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToSuffix as '{header}.BillToSuffix',</v>
       </c>
@@ -3518,7 +3512,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCompany',</v>
       </c>
-      <c r="H61" s="11" t="str">
+      <c r="H61" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCompany as '{header}.BillToCompany',</v>
       </c>
@@ -3548,7 +3542,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCompanyJobTitle',</v>
       </c>
-      <c r="H62" s="11" t="str">
+      <c r="H62" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCompanyJobTitle as '{header}.BillToCompanyJobTitle',</v>
       </c>
@@ -3578,7 +3572,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAttention',</v>
       </c>
-      <c r="H63" s="11" t="str">
+      <c r="H63" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAttention as '{header}.BillToAttention',</v>
       </c>
@@ -3608,7 +3602,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAddressLine1',</v>
       </c>
-      <c r="H64" s="11" t="str">
+      <c r="H64" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine1 as '{header}.BillToAddressLine1',</v>
       </c>
@@ -3638,7 +3632,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAddressLine2',</v>
       </c>
-      <c r="H65" s="11" t="str">
+      <c r="H65" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine2 as '{header}.BillToAddressLine2',</v>
       </c>
@@ -3668,7 +3662,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToAddressLine3',</v>
       </c>
-      <c r="H66" s="11" t="str">
+      <c r="H66" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine3 as '{header}.BillToAddressLine3',</v>
       </c>
@@ -3698,7 +3692,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCity',</v>
       </c>
-      <c r="H67" s="11" t="str">
+      <c r="H67" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCity as '{header}.BillToCity',</v>
       </c>
@@ -3728,7 +3722,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToState',</v>
       </c>
-      <c r="H68" s="11" t="str">
+      <c r="H68" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToState as '{header}.BillToState',</v>
       </c>
@@ -3758,7 +3752,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToStateFullName',</v>
       </c>
-      <c r="H69" s="11" t="str">
+      <c r="H69" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToStateFullName as '{header}.BillToStateFullName',</v>
       </c>
@@ -3788,7 +3782,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToPostalCode',</v>
       </c>
-      <c r="H70" s="11" t="str">
+      <c r="H70" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToPostalCode as '{header}.BillToPostalCode',</v>
       </c>
@@ -3818,7 +3812,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToPostalCodeExt',</v>
       </c>
-      <c r="H71" s="11" t="str">
+      <c r="H71" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToPostalCodeExt as '{header}.BillToPostalCodeExt',</v>
       </c>
@@ -3848,7 +3842,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCounty',</v>
       </c>
-      <c r="H72" s="11" t="str">
+      <c r="H72" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCounty as '{header}.BillToCounty',</v>
       </c>
@@ -3878,7 +3872,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToCountry',</v>
       </c>
-      <c r="H73" s="11" t="str">
+      <c r="H73" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCountry as '{header}.BillToCountry',</v>
       </c>
@@ -3908,7 +3902,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToEmail',</v>
       </c>
-      <c r="H74" s="11" t="str">
+      <c r="H74" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToEmail as '{header}.BillToEmail',</v>
       </c>
@@ -3938,7 +3932,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToDaytimePhone',</v>
       </c>
-      <c r="H75" s="11" t="str">
+      <c r="H75" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToDaytimePhone as '{header}.BillToDaytimePhone',</v>
       </c>
@@ -3968,7 +3962,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.BillToNightPhone',</v>
       </c>
-      <c r="H76" s="11" t="str">
+      <c r="H76" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToNightPhone as '{header}.BillToNightPhone',</v>
       </c>
@@ -4000,7 +3994,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.SignatureFlag',</v>
       </c>
-      <c r="H77" s="11" t="str">
+      <c r="H77" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{Helper.TableAllies}.SignatureFlag as '{header}.SignatureFlag',</v>
       </c>
@@ -4032,7 +4026,7 @@
         <f t="shared" si="2"/>
         <v>as '{header}.ShipmentCount',</v>
       </c>
-      <c r="H78" s="11" t="str">
+      <c r="H78" s="12" t="str">
         <f t="shared" si="3"/>
         <v>{Helper.TableAllies}.ShipmentCount as '{header}.ShipmentCount',</v>
       </c>
@@ -4132,21 +4126,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.6666666666667" customWidth="1"/>
-    <col min="2" max="2" width="35.6666666666667" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="31.4444444444444" customWidth="1"/>
-    <col min="5" max="5" width="2.22222222222222" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="31.4444444444444" customWidth="1"/>
-    <col min="7" max="7" width="30.7777777777778" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="60.1111111111111" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="35.6666666666667" customWidth="1"/>
+    <col min="3" max="3" width="31.4444444444444" customWidth="1"/>
+    <col min="4" max="6" width="32.1111111111111" customWidth="1"/>
+    <col min="7" max="7" width="35.3333333333333" customWidth="1"/>
+    <col min="8" max="8" width="62.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -4195,27 +4187,25 @@
         <v>113</v>
       </c>
       <c r="G3" t="str">
-        <f>REPLACE(E3,12,1,F3)</f>
-        <v>as '{item}.OriginalLineId',</v>
+        <f>REPLACE(E3,5,1,F3)</f>
+        <v>as 'OriginalLineId',</v>
       </c>
       <c r="H3" t="str">
         <f>_xlfn.CONCAT(B3,C3," ",G3)</f>
-        <v>{ItemHelper.TableAllies}.OriginalLineId as '{item}.OriginalLineId',</v>
-      </c>
-    </row>
-    <row r="4" ht="151.2" spans="1:8">
+        <v>{ItemHelper.TableAllies}.OriginalLineId as 'OriginalLineId',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D4" s="8"/>
       <c r="E4" s="7" t="s">
         <v>114</v>
       </c>
@@ -4223,55 +4213,51 @@
         <v>15</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" ref="G4:G29" si="0">REPLACE(E4,12,1,F4)</f>
-        <v>as '{item}.CentralDatabaseNum',</v>
+        <f>REPLACE(E4,5,1,F4)</f>
+        <v>as 'CentralDatabaseNum',</v>
       </c>
       <c r="H4" t="str">
-        <f t="shared" ref="H4:H29" si="1">_xlfn.CONCAT(B4,C4," ",G4)</f>
-        <v>{ItemHelper.TableAllies}.CentralDatabaseNum as '{item}.CentralDatabaseNum',</v>
-      </c>
-    </row>
-    <row r="5" ht="151.2" spans="1:8">
+        <f>_xlfn.CONCAT(B4,C4," ",G4)</f>
+        <v>{OrderLineHelper.TableAllies}.DatabaseNum as 'CentralDatabaseNum',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D5" s="6" t="s">
         <v>116</v>
       </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>as '{item}.CentralOrderLineNum',</v>
+        <f>REPLACE(E5,5,1,F5)</f>
+        <v>as 'CentralOrderLineNum',</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.Seq as '{item}.CentralOrderLineNum',</v>
-      </c>
-    </row>
-    <row r="6" ht="151.2" spans="1:8">
+        <f>_xlfn.CONCAT(B5,C5," ",G5)</f>
+        <v>{OrderLineHelper.TableAllies}.CentralOrderLineNum as 'CentralOrderLineNum',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
         <v>114</v>
       </c>
@@ -4279,27 +4265,25 @@
         <v>118</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>as '{item}.CentralProductNum',</v>
+        <f>REPLACE(E6,5,1,F6)</f>
+        <v>as 'CentralProductNum',</v>
       </c>
       <c r="H6" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.CentralProductNum as '{item}.CentralProductNum',</v>
-      </c>
-    </row>
-    <row r="7" ht="151.2" spans="1:8">
+        <f>_xlfn.CONCAT(B6,C6," ",G6)</f>
+        <v>{ProdcutHelper.TableAllies}.CentralProductNum as 'CentralProductNum',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="D7" s="8"/>
       <c r="E7" s="7" t="s">
         <v>114</v>
       </c>
@@ -4307,15 +4291,15 @@
         <v>119</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>as '{item}.ChannelItemID',</v>
+        <f>REPLACE(E7,5,1,F7)</f>
+        <v>as 'ChannelItemID',</v>
       </c>
       <c r="H7" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ChannelItemID as '{item}.ChannelItemID',</v>
-      </c>
-    </row>
-    <row r="8" ht="151.2" spans="1:8">
+        <f>_xlfn.CONCAT(B7,C7," ",G7)</f>
+        <v>{OrderLineHelper.TableAllies}.ChannelItemID as 'ChannelItemID',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -4332,27 +4316,22 @@
         <v>120</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>as '{item}.SKU',</v>
+        <f>REPLACE(E8,5,1,F8)</f>
+        <v>as 'SKU',</v>
       </c>
       <c r="H8" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.SKU as '{item}.SKU',</v>
-      </c>
-    </row>
-    <row r="9" ht="151.2" spans="1:8">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
+        <f>_xlfn.CONCAT(B8,C8," ",G8)</f>
+        <v>{ItemHelper.TableAllies}.SKU as 'SKU',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="E9" s="7" t="s">
         <v>114</v>
       </c>
@@ -4360,24 +4339,25 @@
         <v>121</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>as '{item}.ItemTitle',</v>
+        <f>REPLACE(E9,5,1,F9)</f>
+        <v>as 'UPC',</v>
       </c>
       <c r="H9" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ItemTitle as '{item}.ItemTitle',</v>
-      </c>
-    </row>
-    <row r="10" ht="151.2" spans="1:8">
+        <f>_xlfn.CONCAT(B9,C9," ",G9)</f>
+        <v>{ProdcutHelper.TableAllies}.UPC as 'UPC',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>122</v>
       </c>
+      <c r="D10" s="8"/>
       <c r="E10" s="7" t="s">
         <v>114</v>
       </c>
@@ -4385,15 +4365,15 @@
         <v>122</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>as '{item}.OrderQty',</v>
+        <f t="shared" ref="G10:G30" si="0">REPLACE(E10,5,1,F10)</f>
+        <v>as 'ItemTitle',</v>
       </c>
       <c r="H10" t="str">
-        <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.OrderQty as '{item}.OrderQty',</v>
-      </c>
-    </row>
-    <row r="11" ht="151.2" spans="1:10">
+        <f t="shared" ref="H10:H30" si="1">_xlfn.CONCAT(B10,C10," ",G10)</f>
+        <v>{OrderLineHelper.TableAllies}.ItemTitle as 'ItemTitle',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -4411,15 +4391,14 @@
       </c>
       <c r="G11" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.ShipQty',</v>
+        <v>as 'OrderQty',</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ShipQty as '{item}.ShipQty',</v>
-      </c>
-      <c r="J11" s="3"/>
-    </row>
-    <row r="12" ht="151.2" spans="1:8">
+        <v>{ItemHelper.TableAllies}.OrderQty as 'OrderQty',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -4433,71 +4412,70 @@
         <v>114</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.CancelQty',</v>
+        <v>as 'ShipQty',</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.CancelledQty as '{item}.CancelQty',</v>
-      </c>
-    </row>
-    <row r="13" ht="151.2" spans="1:8">
+        <v>{ItemHelper.TableAllies}.ShipQty as 'ShipQty',</v>
+      </c>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
         <v>112</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.UnitPrice',</v>
+        <v>as 'CancelQty',</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.Price as '{item}.UnitPrice',</v>
-      </c>
-    </row>
-    <row r="14" ht="151.2" spans="1:8">
+        <v>{ItemHelper.TableAllies}.CancelledQty as 'CancelQty',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D14"/>
       <c r="E14" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineItemTaxAmount',</v>
+        <v>as 'UnitPrice',</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.TaxAmount as '{item}.LineItemTaxAmount',</v>
-      </c>
-    </row>
-    <row r="15" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.UnitPrice as 'UnitPrice',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -4505,24 +4483,24 @@
         <v>112</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineShippingAmount',</v>
+        <v>as 'LineItemTaxAmount',</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ShippingAmount as '{item}.LineShippingAmount',</v>
-      </c>
-    </row>
-    <row r="16" ht="151.2" spans="1:8">
+        <v>{ItemHelper.TableAllies}.TaxAmount as 'LineItemTaxAmount',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -4530,24 +4508,24 @@
         <v>112</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineShippingTaxAmount',</v>
+        <v>as 'LineShippingAmount',</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ShippingTaxAmount as '{item}.LineShippingTaxAmount',</v>
-      </c>
-    </row>
-    <row r="17" ht="151.2" spans="1:8">
+        <v>{ItemHelper.TableAllies}.ShippingAmount as 'LineShippingAmount',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
         <v>36</v>
       </c>
@@ -4555,364 +4533,367 @@
         <v>112</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineShippingDiscount',</v>
+        <v>as 'LineShippingTaxAmount',</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LineShippingDiscount as '{item}.LineShippingDiscount',</v>
-      </c>
-    </row>
-    <row r="18" ht="151.2" spans="1:8">
+        <v>{ItemHelper.TableAllies}.ShippingTaxAmount as 'LineShippingTaxAmount',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="D18" s="8"/>
       <c r="E18" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineShippingDiscountTaxAmount',</v>
+        <v>as 'LineShippingDiscount',</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LineShippingDiscountTaxAmount as '{item}.LineShippingDiscountTaxAmount',</v>
-      </c>
-    </row>
-    <row r="19" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LineShippingDiscount as 'LineShippingDiscount',</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D19" s="8"/>
       <c r="E19" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineRecyclingFee',</v>
+        <v>as 'LineShippingDiscountTaxAmount',</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LineRecyclingFee as '{item}.LineRecyclingFee',</v>
-      </c>
-    </row>
-    <row r="20" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LineShippingDiscountTaxAmount as 'LineShippingDiscountTaxAmount',</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="D20" s="8"/>
       <c r="E20" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineGiftMsg',</v>
+        <v>as 'LineRecyclingFee',</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LineGiftMsg as '{item}.LineGiftMsg',</v>
-      </c>
-    </row>
-    <row r="21" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LineRecyclingFee as 'LineRecyclingFee',</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="D21" s="8"/>
       <c r="E21" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineGiftNotes',</v>
+        <v>as 'LineGiftMsg',</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LineGiftNotes as '{item}.LineGiftNotes',</v>
-      </c>
-    </row>
-    <row r="22" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LineGiftMsg as 'LineGiftMsg',</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="D22" s="8"/>
       <c r="E22" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineGiftAmount',</v>
+        <v>as 'LineGiftNotes',</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LineGiftAmount as '{item}.LineGiftAmount',</v>
-      </c>
-    </row>
-    <row r="23" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LineGiftNotes as 'LineGiftNotes',</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="D23" s="8"/>
       <c r="E23" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LineGiftTaxAmount',</v>
+        <v>as 'LineGiftAmount',</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LineGiftTaxAmount as '{item}.LineGiftTaxAmount',</v>
-      </c>
-    </row>
-    <row r="24" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LineGiftAmount as 'LineGiftAmount',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LinePromotionCodes',</v>
+        <v>as 'LineGiftTaxAmount',</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LinePromotionCodes as '{item}.LinePromotionCodes',</v>
-      </c>
-    </row>
-    <row r="25" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LineGiftTaxAmount as 'LineGiftTaxAmount',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LinePromotionAmount',</v>
+        <v>as 'LinePromotionCodes',</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LinePromotionAmount as '{item}.LinePromotionAmount',</v>
-      </c>
-    </row>
-    <row r="26" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LinePromotionCodes as 'LinePromotionCodes',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D26" s="8"/>
       <c r="E26" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.LinePromotionTaxAmount',</v>
+        <v>as 'LinePromotionAmount',</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.LinePromotionTaxAmount as '{item}.LinePromotionTaxAmount',</v>
-      </c>
-    </row>
-    <row r="27" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LinePromotionAmount as 'LinePromotionAmount',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" s="8"/>
       <c r="E27" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.BundleType',</v>
+        <v>as 'LinePromotionTaxAmount',</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.BundleType as '{item}.BundleType',</v>
-      </c>
-    </row>
-    <row r="28" ht="151.2" spans="1:8">
+        <v>{OrderLineHelper.TableAllies}.LinePromotionTaxAmount as 'LinePromotionTaxAmount',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="8"/>
       <c r="E28" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.BundleItemFulfilmentLineNum',</v>
+        <v>as 'BundleType',</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.BundleItemFulfilmentLineNum as '{item}.BundleItemFulfilmentLineNum',</v>
-      </c>
-    </row>
-    <row r="29" ht="151.2" spans="1:8">
+        <v>{ProdcutHelper.TableAllies}.BundleType as 'BundleType',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
         <v>112</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D29" t="s">
-        <v>145</v>
+        <v>142</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E29" s="7" t="s">
         <v>114</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v>as '{item}.EnterDate',</v>
+        <v>as 'BundleItemFulfilmentLineNum',</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v>{ItemHelper.TableAllies}.ItemDate as '{item}.EnterDate',</v>
+        <v>{ItemHelper.TableAllies}.BundleItemFulfilmentLineNum as 'BundleItemFulfilmentLineNum',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>as 'EnterDate',</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="1"/>
+        <v>{ItemHelper.TableAllies}.ItemDate as 'EnterDate',</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D29">
+  <autoFilter ref="B1:B30">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Add comment to mapping file.
</commit_message>
<xml_diff>
--- a/payload/wms connector/salesorder/SalesOrder mapping.xlsx
+++ b/payload/wms connector/salesorder/SalesOrder mapping.xlsx
@@ -1,25 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BolanYou\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D83E3FAA-8B4F-42FF-BC88-B95135CCF5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9420" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order header" sheetId="4" r:id="rId1"/>
     <sheet name="orderitem" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Order header'!$D$1:$D$78</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">orderitem!$B$1:$B$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Order header'!$A$1:$J$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">orderitem!$D$1:$D$30</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="149">
   <si>
     <t>column type</t>
   </si>
@@ -79,9 +96,6 @@
     <t>WarehouseNum</t>
   </si>
   <si>
-    <t>not exist</t>
-  </si>
-  <si>
     <t>DatabaseNum</t>
   </si>
   <si>
@@ -271,36 +285,24 @@
     <t>LatestShipDate</t>
   </si>
   <si>
-    <t xml:space="preserve">this is supplied by wms </t>
-  </si>
-  <si>
     <t>DeliverByDate</t>
   </si>
   <si>
     <t>ShippingCarrier</t>
   </si>
   <si>
-    <t>ShippingCarrier as RequestShippingCarrier</t>
-  </si>
-  <si>
     <t>RequestShippingCarrier</t>
   </si>
   <si>
     <t>ShippingClass</t>
   </si>
   <si>
-    <t>ShippingClass as RequestShippingService</t>
-  </si>
-  <si>
     <t>RequestShippingService</t>
   </si>
   <si>
     <t>MappedShippingCarrier</t>
   </si>
   <si>
-    <t>wms fill up</t>
-  </si>
-  <si>
     <t>MappedShippingService</t>
   </si>
   <si>
@@ -430,28 +432,6 @@
     <t>ShipmentCount</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF3B4151"/>
-        <rFont val="Courier New"/>
-        <charset val="134"/>
-      </rPr>
-      <t>not exist</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF3B4151"/>
-        <rFont val="SimSun"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>SalesOrderItemsUuid</t>
   </si>
   <si>
@@ -564,23 +544,32 @@
   </si>
   <si>
     <t>EnterDate</t>
+  </si>
+  <si>
+    <t>Ingore or zero</t>
+  </si>
+  <si>
+    <t>Need to find out</t>
+  </si>
+  <si>
+    <t>Ignore</t>
+  </si>
+  <si>
+    <t>Ingore</t>
+  </si>
+  <si>
+    <t>WMS add</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="30">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -588,7 +577,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -602,7 +591,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -640,165 +629,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF606060"/>
       <name val="Courier New"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF3B4151"/>
-      <name val="SimSun"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -817,200 +655,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1033,255 +679,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1318,12 +722,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1339,65 +737,24 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1684,34 +1041,35 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C$1:C$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="34.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="34.8888888888889" customWidth="1"/>
-    <col min="4" max="4" width="47.5555555555556" customWidth="1"/>
-    <col min="5" max="5" width="23.1111111111111" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7777777777778" customWidth="1"/>
-    <col min="7" max="7" width="40.8888888888889" customWidth="1"/>
-    <col min="8" max="8" width="70.6666666666667" style="4" customWidth="1"/>
-    <col min="9" max="9" width="17.2222222222222" customWidth="1"/>
-    <col min="10" max="10" width="29.3333333333333" customWidth="1"/>
-    <col min="11" max="11" width="40.3333333333333" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="70.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" customWidth="1"/>
+    <col min="11" max="11" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1728,7 +1086,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="25.2" customHeight="1" spans="1:10">
+    <row r="2" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1753,12 +1111,12 @@
         <f>_xlfn.CONCAT(B2,C2," ",G2)</f>
         <v>{InfoHelper.TableAllies}.SalesOrderUuid as '{header}.SalesOrderUuid',</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I2" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1783,12 +1141,12 @@
         <f>_xlfn.CONCAT(B3,C3," ",G3)</f>
         <v>{InfoHelper.TableAllies}.WarehouseCode as '{header}.WarehouseCode',</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I3" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" ht="25.15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1799,7 +1157,7 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>8</v>
@@ -1815,12 +1173,12 @@
         <f t="shared" ref="H4:H35" si="1">_xlfn.CONCAT(B4,C4," ",G4)</f>
         <v>{Helper.TableAllies}.WarehouseNum as '{header}.WarehouseNum',</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" ht="37.8" customHeight="1" spans="1:10">
+      <c r="J4" s="17"/>
+    </row>
+    <row r="5" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -1828,14 +1186,14 @@
         <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1845,27 +1203,27 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DatabaseNum as '{header}.CentralDatabaseNum',</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" ht="25.2" customHeight="1" spans="1:10">
+      <c r="J5" s="17"/>
+    </row>
+    <row r="6" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1875,12 +1233,12 @@
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.CentralOrderNum as '{header}.CentralOrderNum',</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="17"/>
+    </row>
+    <row r="7" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1888,14 +1246,14 @@
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1905,12 +1263,12 @@
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelNum as '{header}.ChannelNum',</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" ht="37.8" customHeight="1" spans="1:10">
+      <c r="J7" s="17"/>
+    </row>
+    <row r="8" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1918,14 +1276,14 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1935,27 +1293,27 @@
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelAccountNum as '{header}.ChannelAccountNum',</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" ht="37.8" customHeight="1" spans="1:10">
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1965,12 +1323,12 @@
         <f t="shared" si="1"/>
         <v>channelAccount.ChannelAccountName as '{header}.ChannelAccountName',</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1978,14 +1336,14 @@
         <v>6</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1995,12 +1353,12 @@
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ChannelOrderId as '{header}.ChannelOrderId',</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="17"/>
+    </row>
+    <row r="11" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -2008,14 +1366,14 @@
         <v>6</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2025,12 +1383,12 @@
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.SecondaryChannelOrderId as '{header}.SecondaryChannelOrderId',</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I11" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="17"/>
+    </row>
+    <row r="12" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -2038,14 +1396,14 @@
         <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2055,12 +1413,12 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.OrderNumber as '{header}.SellerOrderId',</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" customHeight="1" spans="1:10">
+      <c r="I12" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="17"/>
+    </row>
+    <row r="13" spans="1:10" ht="14.45" hidden="1" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -2068,14 +1426,14 @@
         <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2085,27 +1443,27 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.Currency as '{header}.Currency',</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I13" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2115,29 +1473,29 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.OrderDate as '{header}.OriginalOrderDate',</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I14" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="E15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="G15" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2147,27 +1505,27 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.SellerPublicNote as '{header}.SellerPublicNotes',</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I15" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="G16" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2177,29 +1535,29 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.SellerPrivateNote as '{header}.SellerPrivateNotes',</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I16" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="17"/>
+    </row>
+    <row r="17" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G17" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2209,27 +1567,27 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.EndBuyerInstruction as '{header}.EndBuyerInstruction',</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I17" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="17"/>
+    </row>
+    <row r="18" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G18" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2239,27 +1597,27 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TotalAmount as '{header}.TotalOrderAmount',</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2269,27 +1627,27 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.TaxAmount as '{header}.TotalTaxAmount',</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2299,27 +1657,27 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.ShippingAmount as '{header}.TotalShippingAmount',</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I20" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2329,27 +1687,27 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.ShippingTaxAmount as '{header}.TotalShippingTaxAmount',</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I21" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="9"/>
       <c r="E22" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2359,27 +1717,27 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.TotalShippingDiscount as '{header}.TotalShippingDiscount',</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" ht="50.4" customHeight="1" spans="1:10">
+      <c r="I22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:10" ht="50.45" hidden="1" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="9"/>
       <c r="E23" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G23" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2389,27 +1747,27 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.TotalShippingDiscountTaxAmount as '{header}.TotalShippingDiscountTaxAmount',</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I23" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="9"/>
       <c r="E24" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G24" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2419,27 +1777,27 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.TotalInsuranceAmount as '{header}.TotalInsuranceAmount',</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="9"/>
       <c r="E25" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G25" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2449,27 +1807,27 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.TotalGiftOptionAmount as '{header}.TotalGiftOptionAmount',</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="9"/>
       <c r="E26" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G26" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2479,29 +1837,29 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.TotalGiftOptionTaxAmount as '{header}.TotalGiftOptionTaxAmount',</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I26" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G27" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2511,57 +1869,57 @@
         <f t="shared" si="1"/>
         <v>{OrderHeaderHelper.TableAllies}.AdditionalCostOrDiscount as '{header}.AdditionalCostOrDiscount',</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" s="8" customFormat="1" ht="25.2" customHeight="1" spans="1:10">
-      <c r="A28" s="14" t="s">
-        <v>37</v>
+      <c r="I27" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="J27" s="17"/>
+    </row>
+    <row r="28" spans="1:10" s="8" customFormat="1" ht="25.15" hidden="1" customHeight="1">
+      <c r="A28" s="12" t="s">
+        <v>36</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28" s="9" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.PromotionAmount',</v>
       </c>
-      <c r="H28" s="15" t="str">
+      <c r="H28" s="13" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DiscountAmount as '{header}.PromotionAmount',</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I28" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="G29" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2571,29 +1929,29 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.ShipDate as '{header}.EstimatedShipDate',</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I29" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="17"/>
+    </row>
+    <row r="30" spans="1:10" ht="25.15" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>13</v>
+      <c r="C30" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>145</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2603,29 +1961,29 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.EarliestShipDate as '{header}.EarliestShipDate',</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I30" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="31" spans="1:10" ht="25.15" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>58</v>
+      <c r="C31" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>145</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G31" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2635,29 +1993,29 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.LatestShipDate as '{header}.LatestShipDate',</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I31" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" ht="25.15" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>58</v>
+      <c r="C32" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>145</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G32" s="7" t="str">
         <f t="shared" si="0"/>
@@ -2667,140 +2025,136 @@
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.DeliverByDate as '{header}.DeliverByDate',</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" s="8" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A33" s="14" t="s">
+      <c r="I32" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="J32" s="17"/>
+    </row>
+    <row r="33" spans="1:10" s="8" customFormat="1" ht="37.9" hidden="1" customHeight="1">
+      <c r="A33" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>61</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D33" s="9"/>
       <c r="E33" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G33" s="9" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.RequestShippingCarrier',</v>
       </c>
-      <c r="H33" s="15" t="str">
+      <c r="H33" s="13" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ShippingCarrier as '{header}.RequestShippingCarrier',</v>
       </c>
-      <c r="I33" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" s="8" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A34" s="14" t="s">
+      <c r="I33" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J33" s="18"/>
+    </row>
+    <row r="34" spans="1:10" s="8" customFormat="1" ht="37.9" hidden="1" customHeight="1">
+      <c r="A34" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>64</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D34" s="9"/>
       <c r="E34" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G34" s="9" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.RequestShippingService',</v>
       </c>
-      <c r="H34" s="15" t="str">
+      <c r="H34" s="13" t="str">
         <f t="shared" si="1"/>
         <v>{InfoHelper.TableAllies}.ShippingClass as '{header}.RequestShippingService',</v>
       </c>
-      <c r="I34" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" s="14"/>
-    </row>
-    <row r="35" s="8" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A35" s="14" t="s">
+      <c r="I34" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J34" s="18"/>
+    </row>
+    <row r="35" spans="1:10" s="8" customFormat="1" ht="37.9" customHeight="1">
+      <c r="A35" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>67</v>
+      <c r="C35" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G35" s="9" t="str">
         <f t="shared" si="0"/>
         <v>as '{header}.MappedShippingCarrier',</v>
       </c>
-      <c r="H35" s="15" t="str">
+      <c r="H35" s="13" t="str">
         <f t="shared" si="1"/>
         <v>{Helper.TableAllies}.MappedShippingCarrier as '{header}.MappedShippingCarrier',</v>
       </c>
-      <c r="I35" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="14"/>
-    </row>
-    <row r="36" s="8" customFormat="1" ht="37.8" customHeight="1" spans="1:10">
-      <c r="A36" s="14" t="s">
+      <c r="I35" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="1:10" s="8" customFormat="1" ht="37.9" customHeight="1">
+      <c r="A36" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>67</v>
+      <c r="C36" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>147</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G36" s="9" t="str">
         <f t="shared" ref="G36:G78" si="2">REPLACE(E36,14,1,F36)</f>
         <v>as '{header}.MappedShippingService',</v>
       </c>
-      <c r="H36" s="15" t="str">
+      <c r="H36" s="13" t="str">
         <f t="shared" ref="H36:H78" si="3">_xlfn.CONCAT(B36,C36," ",G36)</f>
         <v>{Helper.TableAllies}.MappedShippingService as '{header}.MappedShippingService',</v>
       </c>
-      <c r="I36" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J36" s="14"/>
-    </row>
-    <row r="37" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I36" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="J36" s="18"/>
+    </row>
+    <row r="37" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
@@ -2808,14 +2162,14 @@
         <v>6</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G37" s="7" t="str">
         <f t="shared" si="2"/>
@@ -2825,12 +2179,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToName as '{header}.ShipToName',</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I37" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J37" s="17"/>
+    </row>
+    <row r="38" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
@@ -2838,14 +2192,14 @@
         <v>6</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G38" s="7" t="str">
         <f t="shared" si="2"/>
@@ -2855,12 +2209,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToFirstName as '{header}.ShipToFirstName',</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I38" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
@@ -2868,14 +2222,14 @@
         <v>6</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G39" s="7" t="str">
         <f t="shared" si="2"/>
@@ -2885,12 +2239,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToLastName as '{header}.ShipToLastName',</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I39" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -2898,14 +2252,14 @@
         <v>6</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G40" s="7" t="str">
         <f t="shared" si="2"/>
@@ -2915,12 +2269,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToSuffix as '{header}.ShipToSuffix',</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I40" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>5</v>
       </c>
@@ -2928,14 +2282,14 @@
         <v>6</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G41" s="7" t="str">
         <f t="shared" si="2"/>
@@ -2945,12 +2299,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCompany as '{header}.ShipToCompany',</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I41" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J41" s="17"/>
+    </row>
+    <row r="42" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>5</v>
       </c>
@@ -2958,14 +2312,14 @@
         <v>6</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G42" s="7" t="str">
         <f t="shared" si="2"/>
@@ -2975,12 +2329,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCompanyJobTitle as '{header}.ShipToCompanyJobTitle',</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I42" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J42" s="17"/>
+    </row>
+    <row r="43" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
@@ -2988,14 +2342,14 @@
         <v>6</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="G43" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3005,12 +2359,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAttention as '{header}.ShipToAttention',</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I43" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
@@ -3018,14 +2372,14 @@
         <v>6</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G44" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3035,12 +2389,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToDaytimePhone as '{header}.ShipToDaytimePhone',</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I44" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44" s="17"/>
+    </row>
+    <row r="45" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>5</v>
       </c>
@@ -3048,14 +2402,14 @@
         <v>6</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G45" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3065,12 +2419,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToNightPhone as '{header}.ShipToNightPhone',</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I45" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J45" s="17"/>
+    </row>
+    <row r="46" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
@@ -3078,14 +2432,14 @@
         <v>6</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G46" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3095,12 +2449,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine1 as '{header}.ShipToAddressLine1',</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I46" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J46" s="17"/>
+    </row>
+    <row r="47" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -3108,14 +2462,14 @@
         <v>6</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G47" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3125,12 +2479,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine2 as '{header}.ShipToAddressLine2',</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I47" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
@@ -3138,14 +2492,14 @@
         <v>6</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G48" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3155,12 +2509,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToAddressLine3 as '{header}.ShipToAddressLine3',</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I48" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J48" s="17"/>
+    </row>
+    <row r="49" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -3168,14 +2522,14 @@
         <v>6</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G49" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3185,12 +2539,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCity as '{header}.ShipToCity',</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J49" s="2"/>
-    </row>
-    <row r="50" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I49" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J49" s="17"/>
+    </row>
+    <row r="50" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -3198,14 +2552,14 @@
         <v>6</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G50" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3215,12 +2569,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToState as '{header}.ShipToState',</v>
       </c>
-      <c r="I50" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J50" s="2"/>
-    </row>
-    <row r="51" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I50" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" s="17"/>
+    </row>
+    <row r="51" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
@@ -3228,14 +2582,14 @@
         <v>6</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D51" s="7"/>
       <c r="E51" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G51" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3245,12 +2599,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToStateFullName as '{header}.ShipToStateFullName',</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="52" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I51" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J51" s="17"/>
+    </row>
+    <row r="52" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
@@ -3258,14 +2612,14 @@
         <v>6</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G52" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3275,12 +2629,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToPostalCode as '{header}.ShipToPostalCode',</v>
       </c>
-      <c r="I52" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J52" s="2"/>
-    </row>
-    <row r="53" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I52" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J52" s="17"/>
+    </row>
+    <row r="53" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
@@ -3288,14 +2642,14 @@
         <v>6</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G53" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3305,12 +2659,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToPostalCodeExt as '{header}.ShipToPostalCodeExt',</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J53" s="2"/>
-    </row>
-    <row r="54" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I53" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J53" s="17"/>
+    </row>
+    <row r="54" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
@@ -3318,14 +2672,14 @@
         <v>6</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G54" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3335,12 +2689,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCounty as '{header}.ShipToCounty',</v>
       </c>
-      <c r="I54" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="55" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I54" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J54" s="17"/>
+    </row>
+    <row r="55" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A55" s="2" t="s">
         <v>5</v>
       </c>
@@ -3348,14 +2702,14 @@
         <v>6</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G55" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3365,12 +2719,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToCountry as '{header}.ShipToCountry',</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J55" s="2"/>
-    </row>
-    <row r="56" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I55" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J55" s="17"/>
+    </row>
+    <row r="56" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
@@ -3378,14 +2732,14 @@
         <v>6</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G56" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3395,12 +2749,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.ShipToEmail as '{header}.ShipToEmail',</v>
       </c>
-      <c r="I56" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J56" s="2"/>
-    </row>
-    <row r="57" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I56" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J56" s="17"/>
+    </row>
+    <row r="57" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
@@ -3408,14 +2762,14 @@
         <v>6</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G57" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3425,12 +2779,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToName as '{header}.BillToName',</v>
       </c>
-      <c r="I57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="58" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I57" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J57" s="17"/>
+    </row>
+    <row r="58" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -3438,14 +2792,14 @@
         <v>6</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G58" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3455,12 +2809,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToFirstName as '{header}.BillToFirstName',</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J58" s="2"/>
-    </row>
-    <row r="59" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I58" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J58" s="17"/>
+    </row>
+    <row r="59" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>5</v>
       </c>
@@ -3468,14 +2822,14 @@
         <v>6</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G59" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3485,12 +2839,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToLastName as '{header}.BillToLastName',</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J59" s="2"/>
-    </row>
-    <row r="60" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I59" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" s="17"/>
+    </row>
+    <row r="60" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
@@ -3498,14 +2852,14 @@
         <v>6</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G60" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3515,12 +2869,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToSuffix as '{header}.BillToSuffix',</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="61" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I60" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J60" s="17"/>
+    </row>
+    <row r="61" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -3528,14 +2882,14 @@
         <v>6</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G61" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3545,12 +2899,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCompany as '{header}.BillToCompany',</v>
       </c>
-      <c r="I61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J61" s="2"/>
-    </row>
-    <row r="62" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I61" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J61" s="17"/>
+    </row>
+    <row r="62" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
@@ -3558,14 +2912,14 @@
         <v>6</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G62" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3575,12 +2929,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCompanyJobTitle as '{header}.BillToCompanyJobTitle',</v>
       </c>
-      <c r="I62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J62" s="2"/>
-    </row>
-    <row r="63" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I62" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J62" s="17"/>
+    </row>
+    <row r="63" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>5</v>
       </c>
@@ -3588,14 +2942,14 @@
         <v>6</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G63" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3605,12 +2959,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAttention as '{header}.BillToAttention',</v>
       </c>
-      <c r="I63" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="64" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I63" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J63" s="17"/>
+    </row>
+    <row r="64" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A64" s="2" t="s">
         <v>5</v>
       </c>
@@ -3618,14 +2972,14 @@
         <v>6</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G64" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3635,12 +2989,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine1 as '{header}.BillToAddressLine1',</v>
       </c>
-      <c r="I64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J64" s="2"/>
-    </row>
-    <row r="65" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I64" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J64" s="17"/>
+    </row>
+    <row r="65" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
@@ -3648,14 +3002,14 @@
         <v>6</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G65" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3665,12 +3019,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine2 as '{header}.BillToAddressLine2',</v>
       </c>
-      <c r="I65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I65" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J65" s="17"/>
+    </row>
+    <row r="66" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A66" s="2" t="s">
         <v>5</v>
       </c>
@@ -3678,14 +3032,14 @@
         <v>6</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G66" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3695,12 +3049,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToAddressLine3 as '{header}.BillToAddressLine3',</v>
       </c>
-      <c r="I66" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I66" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J66" s="17"/>
+    </row>
+    <row r="67" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>5</v>
       </c>
@@ -3708,14 +3062,14 @@
         <v>6</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G67" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3725,12 +3079,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCity as '{header}.BillToCity',</v>
       </c>
-      <c r="I67" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J67" s="2"/>
-    </row>
-    <row r="68" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I67" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J67" s="17"/>
+    </row>
+    <row r="68" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A68" s="2" t="s">
         <v>5</v>
       </c>
@@ -3738,14 +3092,14 @@
         <v>6</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G68" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3755,12 +3109,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToState as '{header}.BillToState',</v>
       </c>
-      <c r="I68" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J68" s="2"/>
-    </row>
-    <row r="69" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I68" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J68" s="17"/>
+    </row>
+    <row r="69" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
@@ -3768,14 +3122,14 @@
         <v>6</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G69" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3785,12 +3139,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToStateFullName as '{header}.BillToStateFullName',</v>
       </c>
-      <c r="I69" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J69" s="2"/>
-    </row>
-    <row r="70" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I69" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J69" s="17"/>
+    </row>
+    <row r="70" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>5</v>
       </c>
@@ -3798,14 +3152,14 @@
         <v>6</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G70" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3815,12 +3169,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToPostalCode as '{header}.BillToPostalCode',</v>
       </c>
-      <c r="I70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J70" s="2"/>
-    </row>
-    <row r="71" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I70" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J70" s="17"/>
+    </row>
+    <row r="71" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>5</v>
       </c>
@@ -3828,14 +3182,14 @@
         <v>6</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G71" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3845,12 +3199,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToPostalCodeExt as '{header}.BillToPostalCodeExt',</v>
       </c>
-      <c r="I71" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J71" s="2"/>
-    </row>
-    <row r="72" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I71" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J71" s="17"/>
+    </row>
+    <row r="72" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -3858,14 +3212,14 @@
         <v>6</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G72" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3875,12 +3229,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCounty as '{header}.BillToCounty',</v>
       </c>
-      <c r="I72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J72" s="2"/>
-    </row>
-    <row r="73" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I72" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J72" s="17"/>
+    </row>
+    <row r="73" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>5</v>
       </c>
@@ -3888,14 +3242,14 @@
         <v>6</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G73" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3905,12 +3259,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToCountry as '{header}.BillToCountry',</v>
       </c>
-      <c r="I73" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J73" s="2"/>
-    </row>
-    <row r="74" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I73" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J73" s="17"/>
+    </row>
+    <row r="74" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>5</v>
       </c>
@@ -3918,14 +3272,14 @@
         <v>6</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G74" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3935,12 +3289,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToEmail as '{header}.BillToEmail',</v>
       </c>
-      <c r="I74" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J74" s="2"/>
-    </row>
-    <row r="75" ht="37.8" customHeight="1" spans="1:10">
+      <c r="I74" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J74" s="17"/>
+    </row>
+    <row r="75" spans="1:10" ht="37.9" hidden="1" customHeight="1">
       <c r="A75" s="2" t="s">
         <v>5</v>
       </c>
@@ -3948,14 +3302,14 @@
         <v>6</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G75" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3965,12 +3319,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToDaytimePhone as '{header}.BillToDaytimePhone',</v>
       </c>
-      <c r="I75" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J75" s="2"/>
-    </row>
-    <row r="76" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I75" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J75" s="17"/>
+    </row>
+    <row r="76" spans="1:10" ht="25.15" hidden="1" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>5</v>
       </c>
@@ -3978,14 +3332,14 @@
         <v>6</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G76" s="7" t="str">
         <f t="shared" si="2"/>
@@ -3995,12 +3349,12 @@
         <f t="shared" si="3"/>
         <v>{InfoHelper.TableAllies}.BillToNightPhone as '{header}.BillToNightPhone',</v>
       </c>
-      <c r="I76" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J76" s="2"/>
-    </row>
-    <row r="77" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I76" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J76" s="17"/>
+    </row>
+    <row r="77" spans="1:10" ht="25.15" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>5</v>
       </c>
@@ -4008,16 +3362,16 @@
         <v>11</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="E77" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F77" s="7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G77" s="7" t="str">
         <f t="shared" si="2"/>
@@ -4027,12 +3381,12 @@
         <f t="shared" si="3"/>
         <v>{Helper.TableAllies}.SignatureFlag as '{header}.SignatureFlag',</v>
       </c>
-      <c r="I77" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J77" s="2"/>
-    </row>
-    <row r="78" ht="25.2" customHeight="1" spans="1:10">
+      <c r="I77" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J77" s="17"/>
+    </row>
+    <row r="78" spans="1:10" ht="25.15" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>10</v>
       </c>
@@ -4040,16 +3394,16 @@
         <v>11</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E78" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G78" s="7" t="str">
         <f t="shared" si="2"/>
@@ -4059,120 +3413,123 @@
         <f t="shared" si="3"/>
         <v>{Helper.TableAllies}.ShipmentCount as '{header}.ShipmentCount',</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="I78" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="J78" s="2"/>
+      <c r="J78" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D78">
-    <extLst/>
+  <autoFilter ref="A1:J78" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
   </autoFilter>
   <mergeCells count="77">
+    <mergeCell ref="I77:J77"/>
+    <mergeCell ref="I78:J78"/>
+    <mergeCell ref="I72:J72"/>
+    <mergeCell ref="I73:J73"/>
+    <mergeCell ref="I74:J74"/>
+    <mergeCell ref="I75:J75"/>
+    <mergeCell ref="I76:J76"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="I70:J70"/>
+    <mergeCell ref="I71:J71"/>
+    <mergeCell ref="I62:J62"/>
+    <mergeCell ref="I63:J63"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I59:J59"/>
+    <mergeCell ref="I60:J60"/>
+    <mergeCell ref="I61:J61"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="I54:J54"/>
+    <mergeCell ref="I55:J55"/>
+    <mergeCell ref="I56:J56"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="I33:J33"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="I32:J32"/>
-    <mergeCell ref="I33:J33"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="I36:J36"/>
-    <mergeCell ref="I37:J37"/>
-    <mergeCell ref="I38:J38"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
-    <mergeCell ref="I51:J51"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I53:J53"/>
-    <mergeCell ref="I54:J54"/>
-    <mergeCell ref="I55:J55"/>
-    <mergeCell ref="I56:J56"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="I58:J58"/>
-    <mergeCell ref="I59:J59"/>
-    <mergeCell ref="I60:J60"/>
-    <mergeCell ref="I61:J61"/>
-    <mergeCell ref="I62:J62"/>
-    <mergeCell ref="I63:J63"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I72:J72"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="I74:J74"/>
-    <mergeCell ref="I75:J75"/>
-    <mergeCell ref="I76:J76"/>
-    <mergeCell ref="I77:J77"/>
-    <mergeCell ref="I78:J78"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="35.6666666666667" customWidth="1"/>
-    <col min="3" max="3" width="36.3333333333333" customWidth="1"/>
-    <col min="4" max="4" width="29.7777777777778" customWidth="1"/>
-    <col min="5" max="5" width="13.6666666666667" customWidth="1"/>
-    <col min="6" max="6" width="32.4444444444444" customWidth="1"/>
-    <col min="7" max="7" width="35.3333333333333" customWidth="1"/>
-    <col min="8" max="8" width="62.7777777777778" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="62.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4189,33 +3546,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" ht="16" customHeight="1" spans="1:8">
+    <row r="3" spans="1:10" ht="15.95" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>13</v>
+        <v>146</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G9" si="0">REPLACE(E3,5,1,F3)</f>
@@ -4226,22 +3586,22 @@
         <v>{ItemHelper.TableAllies}.OriginalLineId as 'OriginalLineId',</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="0"/>
@@ -4252,22 +3612,22 @@
         <v>{OrderLineHelper.TableAllies}.DatabaseNum as 'CentralDatabaseNum',</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10" ht="25.5">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="0"/>
@@ -4278,22 +3638,22 @@
         <v>{OrderLineHelper.TableAllies}.CentralOrderLineNum as 'CentralOrderLineNum',</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="0"/>
@@ -4304,22 +3664,22 @@
         <v>{ProdcutHelper.TableAllies}.CentralProductNum as 'CentralProductNum',</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="0"/>
@@ -4330,21 +3690,21 @@
         <v>{OrderLineHelper.TableAllies}.ChannelItemID as 'ChannelItemID',</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E8" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>121</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="0"/>
@@ -4355,19 +3715,19 @@
         <v>{ItemHelper.TableAllies}.SKU as 'SKU',</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="0"/>
@@ -4378,22 +3738,22 @@
         <v>{ProdcutHelper.TableAllies}.UPC as 'UPC',</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" ref="G10:G30" si="2">REPLACE(E10,5,1,F10)</f>
@@ -4404,21 +3764,21 @@
         <v>{ProdcutHelper.TableAllies}.ProductTitle as 'ItemTitle',</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="2"/>
@@ -4434,16 +3794,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="2"/>
@@ -4455,21 +3815,21 @@
       </c>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="2"/>
@@ -4480,21 +3840,21 @@
         <v>{ItemHelper.TableAllies}.CancelledQty as 'CancelQty',</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="2"/>
@@ -4505,21 +3865,21 @@
         <v>{ItemHelper.TableAllies}.Price as 'UnitPrice',</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="2"/>
@@ -4530,21 +3890,21 @@
         <v>{ItemHelper.TableAllies}.TaxAmount as 'LineItemTaxAmount',</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="2"/>
@@ -4557,19 +3917,19 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="2"/>
@@ -4580,22 +3940,22 @@
         <v>{ItemHelper.TableAllies}.ShippingTaxAmount as 'LineShippingTaxAmount',</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="25.5">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="2"/>
@@ -4606,22 +3966,22 @@
         <v>{OrderLineHelper.TableAllies}.LineShippingDiscount as 'LineShippingDiscount',</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="25.5">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="2"/>
@@ -4634,20 +3994,20 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="2"/>
@@ -4663,17 +4023,17 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="2"/>
@@ -4689,17 +4049,17 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="2"/>
@@ -4712,20 +4072,20 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="2"/>
@@ -4738,20 +4098,20 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D24" s="8"/>
       <c r="E24" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="2"/>
@@ -4762,22 +4122,22 @@
         <v>{ItemHelper.TableAllies}.MiscTaxAmount as 'LineGiftTaxAmount',</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="25.5">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="2"/>
@@ -4790,20 +4150,20 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="2"/>
@@ -4814,22 +4174,22 @@
         <v>{ItemHelper.TableAllies}.DiscountAmount as 'LinePromotionAmount',</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="25.5">
       <c r="A27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="2"/>
@@ -4845,17 +4205,17 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="2"/>
@@ -4866,24 +4226,24 @@
         <v>{ProdcutHelper.TableAllies}.BundleType as 'BundleType',</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="25.5">
       <c r="A29" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="E29" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="2"/>
@@ -4894,24 +4254,24 @@
         <v>{ItemHelper.TableAllies}.BundleItemFulfilmentLineNum as 'BundleItemFulfilmentLineNum',</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="25.5">
       <c r="A30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="2"/>
@@ -4923,10 +4283,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B30">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="D1:D30" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add latestshipdate to salesorder header and items.
</commit_message>
<xml_diff>
--- a/payload/wms connector/salesorder/SalesOrder mapping.xlsx
+++ b/payload/wms connector/salesorder/SalesOrder mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="149">
   <si>
     <t>column type</t>
   </si>
@@ -259,19 +259,19 @@
     <t>PromotionAmount</t>
   </si>
   <si>
+    <t>ShipDate</t>
+  </si>
+  <si>
+    <t>EstimatedShipDate</t>
+  </si>
+  <si>
+    <t>EarliestShipDate</t>
+  </si>
+  <si>
+    <t>LatestShipDate</t>
+  </si>
+  <si>
     <t>EtaArrivalDate</t>
-  </si>
-  <si>
-    <t>EstimatedShipDate</t>
-  </si>
-  <si>
-    <t>EarliestShipDate</t>
-  </si>
-  <si>
-    <t>LatestShipDate</t>
-  </si>
-  <si>
-    <t>Need to find out</t>
   </si>
   <si>
     <t>DeliverByDate</t>
@@ -1655,7 +1655,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31:D31"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4"/>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="H29" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>{Helper.TableAllies}.EtaArrivalDate as '{header}.EstimatedShipDate',</v>
+        <v>{Helper.TableAllies}.ShipDate as '{header}.EstimatedShipDate',</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>27</v>
@@ -2575,12 +2575,10 @@
       <c r="B31" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="17" t="s">
-        <v>58</v>
-      </c>
+      <c r="D31" s="16"/>
       <c r="E31" s="7" t="s">
         <v>8</v>
       </c>
@@ -2607,12 +2605,10 @@
       <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>58</v>
       </c>
+      <c r="D32" s="16"/>
       <c r="E32" s="7" t="s">
         <v>8</v>
       </c>
@@ -2625,7 +2621,7 @@
       </c>
       <c r="H32" s="11" t="str">
         <f t="shared" si="1"/>
-        <v>{Helper.TableAllies}.DeliverByDate as '{header}.DeliverByDate',</v>
+        <v>{Helper.TableAllies}.EtaArrivalDate as '{header}.DeliverByDate',</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update mapping file update check saleorder script.
</commit_message>
<xml_diff>
--- a/payload/wms connector/salesorder/SalesOrder mapping.xlsx
+++ b/payload/wms connector/salesorder/SalesOrder mapping.xlsx
@@ -1654,8 +1654,8 @@
   <sheetPr/>
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4"/>

</xml_diff>